<commit_message>
Fixing missing citys: Rio Grande and Loiza
</commit_message>
<xml_diff>
--- a/data/cases2020.xlsx
+++ b/data/cases2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8A1B8-8FD3-0E41-AE3D-7CD46A1ECBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA8324-794D-3340-943C-BA1E42FFB973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="460" windowWidth="12440" windowHeight="16420" xr2:uid="{EA1C0F59-76DC-264A-8C0C-CFD5D20EC04A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15460" windowHeight="16280" xr2:uid="{EA1C0F59-76DC-264A-8C0C-CFD5D20EC04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1451E780-84DC-F94A-879A-A3169D9B97B3}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="158" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>4091</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>2117</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2073</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>1887</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>1240</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -541,7 +541,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>7846</v>
+        <v>7817</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -552,7 +552,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>4191</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>4059</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>3828</v>
+        <v>3836</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>2291</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -607,7 +607,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>5475</v>
+        <v>5480</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>2803</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>2855</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>2394</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <v>1582</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -673,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>885</v>
+        <v>887</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>401</v>
+        <v>761</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>195</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -717,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>228</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>220</v>
+        <v>433</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>111</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="C28">
-        <v>62</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -761,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>3152</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -794,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>1741</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>7</v>
       </c>
       <c r="C34">
-        <v>928</v>
+        <v>930</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -849,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>9658</v>
+        <v>9878</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -860,7 +860,7 @@
         <v>4</v>
       </c>
       <c r="C38">
-        <v>5514</v>
+        <v>5674</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>5341</v>
+        <v>5480</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -882,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>5188</v>
+        <v>5311</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -893,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="C41">
-        <v>3022</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -904,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="C42">
-        <v>1706</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -915,7 +915,7 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>1028</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>2966</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="C45">
-        <v>1499</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -948,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <v>1631</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -959,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>1373</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -970,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="C48">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>